<commit_message>
RDM-4997 Updated definition and feature files to make the mandatory for fixed list on a class rather than class location.
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v15_RDM-4997_fixed_list_order.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v15_RDM-4997_fixed_list_order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/src/ccd/temp/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1811,9 +1811,6 @@
     <t>School regional centre</t>
   </si>
   <si>
-    <t>mandatoryClassForEnum</t>
-  </si>
-  <si>
     <t>BSc</t>
   </si>
   <si>
@@ -1866,6 +1863,9 @@
   </si>
   <si>
     <t>ClassMandatoryFor</t>
+  </si>
+  <si>
+    <t>classMandatoryForEnum</t>
   </si>
 </sst>
 </file>
@@ -2269,7 +2269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2359,21 +2359,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2391,8 +2378,10 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2601,9 +2590,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2618,6 +2608,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
@@ -22481,10 +22473,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:E47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23737,7 +23729,7 @@
         <v>60</v>
       </c>
       <c r="F38" s="158" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G38" s="189" t="s">
         <v>547</v>
@@ -23825,20 +23817,18 @@
         <v>42736</v>
       </c>
       <c r="B41" s="156"/>
-      <c r="C41" s="158" t="s">
-        <v>542</v>
-      </c>
-      <c r="D41" s="192" t="s">
-        <v>580</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="59" t="s">
-        <v>562</v>
-      </c>
+      <c r="C41" s="106" t="s">
+        <v>543</v>
+      </c>
+      <c r="D41" s="189" t="s">
+        <v>535</v>
+      </c>
+      <c r="E41" s="157" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="158"/>
       <c r="G41" s="189" t="s">
-        <v>569</v>
+        <v>536</v>
       </c>
       <c r="H41" s="157"/>
       <c r="I41" s="158"/>
@@ -23863,14 +23853,14 @@
         <v>543</v>
       </c>
       <c r="D42" s="189" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="E42" s="157" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F42" s="158"/>
       <c r="G42" s="189" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="H42" s="157"/>
       <c r="I42" s="158"/>
@@ -23895,14 +23885,14 @@
         <v>543</v>
       </c>
       <c r="D43" s="189" t="s">
-        <v>537</v>
-      </c>
-      <c r="E43" s="157" t="s">
-        <v>48</v>
+        <v>539</v>
+      </c>
+      <c r="E43" s="158" t="s">
+        <v>542</v>
       </c>
       <c r="F43" s="158"/>
       <c r="G43" s="189" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="H43" s="157"/>
       <c r="I43" s="158"/>
@@ -23919,27 +23909,27 @@
       <c r="R43" s="158"/>
     </row>
     <row r="44" spans="1:18" s="160" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="156">
-        <v>42736</v>
-      </c>
-      <c r="B44" s="156"/>
-      <c r="C44" s="106" t="s">
-        <v>543</v>
-      </c>
-      <c r="D44" s="189" t="s">
-        <v>539</v>
-      </c>
-      <c r="E44" s="158" t="s">
-        <v>542</v>
-      </c>
-      <c r="F44" s="158"/>
-      <c r="G44" s="189" t="s">
-        <v>540</v>
-      </c>
-      <c r="H44" s="157"/>
-      <c r="I44" s="158"/>
-      <c r="J44" s="158"/>
-      <c r="K44" s="157" t="s">
+      <c r="A44" s="103">
+        <v>42736</v>
+      </c>
+      <c r="B44" s="103"/>
+      <c r="C44" s="105" t="s">
+        <v>435</v>
+      </c>
+      <c r="D44" s="105" t="s">
+        <v>432</v>
+      </c>
+      <c r="E44" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" s="107"/>
+      <c r="G44" s="105" t="s">
+        <v>433</v>
+      </c>
+      <c r="H44" s="104"/>
+      <c r="I44" s="106"/>
+      <c r="J44" s="106"/>
+      <c r="K44" s="104" t="s">
         <v>27</v>
       </c>
       <c r="L44" s="158"/>
@@ -23959,14 +23949,16 @@
         <v>435</v>
       </c>
       <c r="D45" s="105" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="E45" s="104" t="s">
-        <v>48</v>
-      </c>
-      <c r="F45" s="107"/>
+        <v>64</v>
+      </c>
+      <c r="F45" s="107" t="s">
+        <v>287</v>
+      </c>
       <c r="G45" s="105" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="H45" s="104"/>
       <c r="I45" s="106"/>
@@ -23990,17 +23982,15 @@
       <c r="C46" s="105" t="s">
         <v>435</v>
       </c>
-      <c r="D46" s="105" t="s">
-        <v>438</v>
-      </c>
-      <c r="E46" s="104" t="s">
-        <v>64</v>
-      </c>
-      <c r="F46" s="107" t="s">
-        <v>287</v>
-      </c>
-      <c r="G46" s="105" t="s">
-        <v>441</v>
+      <c r="D46" s="104" t="s">
+        <v>533</v>
+      </c>
+      <c r="E46" s="106" t="s">
+        <v>543</v>
+      </c>
+      <c r="F46" s="106"/>
+      <c r="G46" s="104" t="s">
+        <v>534</v>
       </c>
       <c r="H46" s="104"/>
       <c r="I46" s="106"/>
@@ -24017,27 +24007,29 @@
       <c r="R46" s="158"/>
     </row>
     <row r="47" spans="1:18" s="160" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="103">
-        <v>42736</v>
-      </c>
-      <c r="B47" s="103"/>
-      <c r="C47" s="105" t="s">
+      <c r="A47" s="156">
+        <v>42736</v>
+      </c>
+      <c r="B47" s="192"/>
+      <c r="C47" s="193" t="s">
         <v>435</v>
       </c>
-      <c r="D47" s="104" t="s">
-        <v>533</v>
-      </c>
-      <c r="E47" s="106" t="s">
-        <v>543</v>
-      </c>
-      <c r="F47" s="106"/>
-      <c r="G47" s="104" t="s">
-        <v>534</v>
-      </c>
-      <c r="H47" s="104"/>
-      <c r="I47" s="106"/>
-      <c r="J47" s="106"/>
-      <c r="K47" s="104" t="s">
+      <c r="D47" s="72" t="s">
+        <v>579</v>
+      </c>
+      <c r="E47" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="72" t="s">
+        <v>580</v>
+      </c>
+      <c r="G47" s="72" t="s">
+        <v>568</v>
+      </c>
+      <c r="H47" s="72"/>
+      <c r="I47" s="193"/>
+      <c r="J47" s="193"/>
+      <c r="K47" s="72" t="s">
         <v>27</v>
       </c>
       <c r="L47" s="158"/>
@@ -24080,7 +24072,7 @@
       <c r="Q48" s="158"/>
       <c r="R48" s="158"/>
     </row>
-    <row r="49" spans="1:18" s="101" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" s="160" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="103">
         <v>42736</v>
       </c>
@@ -24104,13 +24096,13 @@
       <c r="K49" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="L49" s="106"/>
-      <c r="M49" s="106"/>
-      <c r="N49" s="106"/>
-      <c r="O49" s="106"/>
-      <c r="P49" s="106"/>
-      <c r="Q49" s="106"/>
-      <c r="R49" s="106"/>
+      <c r="L49" s="158"/>
+      <c r="M49" s="158"/>
+      <c r="N49" s="158"/>
+      <c r="O49" s="158"/>
+      <c r="P49" s="158"/>
+      <c r="Q49" s="158"/>
+      <c r="R49" s="158"/>
     </row>
     <row r="50" spans="1:18" s="101" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="103">
@@ -24178,7 +24170,7 @@
       <c r="Q51" s="106"/>
       <c r="R51" s="106"/>
     </row>
-    <row r="52" spans="1:18" s="160" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" s="101" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="103">
         <v>42736</v>
       </c>
@@ -24187,7 +24179,7 @@
         <v>431</v>
       </c>
       <c r="D52" s="103" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E52" s="104" t="s">
         <v>555</v>
@@ -24204,15 +24196,15 @@
       <c r="K52" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="L52" s="156"/>
-      <c r="M52" s="156"/>
-      <c r="N52" s="156"/>
-      <c r="O52" s="156"/>
-      <c r="P52" s="156"/>
-      <c r="Q52" s="156"/>
-      <c r="R52" s="156"/>
-    </row>
-    <row r="53" spans="1:18" s="101" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L52" s="106"/>
+      <c r="M52" s="106"/>
+      <c r="N52" s="106"/>
+      <c r="O52" s="106"/>
+      <c r="P52" s="106"/>
+      <c r="Q52" s="106"/>
+      <c r="R52" s="106"/>
+    </row>
+    <row r="53" spans="1:18" s="160" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="16"/>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
@@ -24224,13 +24216,13 @@
       <c r="I53" s="16"/>
       <c r="J53" s="16"/>
       <c r="K53" s="16"/>
-      <c r="L53" s="103"/>
-      <c r="M53" s="103"/>
-      <c r="N53" s="103"/>
-      <c r="O53" s="103"/>
-      <c r="P53" s="103"/>
-      <c r="Q53" s="103"/>
-      <c r="R53" s="103"/>
+      <c r="L53" s="156"/>
+      <c r="M53" s="156"/>
+      <c r="N53" s="156"/>
+      <c r="O53" s="156"/>
+      <c r="P53" s="156"/>
+      <c r="Q53" s="156"/>
+      <c r="R53" s="156"/>
     </row>
     <row r="54" spans="1:18" s="101" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="16"/>
@@ -24244,13 +24236,13 @@
       <c r="I54" s="16"/>
       <c r="J54" s="16"/>
       <c r="K54" s="16"/>
-      <c r="L54" s="97"/>
-      <c r="M54" s="97"/>
-      <c r="N54" s="97"/>
-      <c r="O54" s="97"/>
-      <c r="P54" s="97"/>
-      <c r="Q54" s="97"/>
-      <c r="R54" s="97"/>
+      <c r="L54" s="103"/>
+      <c r="M54" s="103"/>
+      <c r="N54" s="103"/>
+      <c r="O54" s="103"/>
+      <c r="P54" s="103"/>
+      <c r="Q54" s="103"/>
+      <c r="R54" s="103"/>
     </row>
     <row r="55" spans="1:18" s="101" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="16"/>
@@ -24271,6 +24263,26 @@
       <c r="P55" s="97"/>
       <c r="Q55" s="97"/>
       <c r="R55" s="97"/>
+    </row>
+    <row r="56" spans="1:18" s="101" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="97"/>
+      <c r="M56" s="97"/>
+      <c r="N56" s="97"/>
+      <c r="O56" s="97"/>
+      <c r="P56" s="97"/>
+      <c r="Q56" s="97"/>
+      <c r="R56" s="97"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -24459,7 +24471,7 @@
         <v>454</v>
       </c>
       <c r="F6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -24815,7 +24827,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:F22"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24988,13 +25000,13 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="8" t="s">
-        <v>562</v>
+        <v>580</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>564</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>565</v>
       </c>
       <c r="F8" s="7">
         <v>4</v>
@@ -25010,13 +25022,13 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="8" t="s">
-        <v>562</v>
+        <v>580</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>566</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>567</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>568</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -25030,13 +25042,13 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>562</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>563</v>
-      </c>
       <c r="E10" s="8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F10" s="7">
         <v>2</v>
@@ -25206,13 +25218,13 @@
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>574</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>570</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>575</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>571</v>
       </c>
       <c r="F19" s="7">
         <v>2</v>
@@ -25224,13 +25236,13 @@
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F20" s="7">
         <v>4</v>
@@ -25242,13 +25254,13 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F21" s="7">
         <v>5</v>
@@ -25260,13 +25272,13 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F22" s="7">
         <v>7</v>

</xml_diff>

<commit_message>
RDM-4997 Updates feature file and definition.
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v15_RDM-4997_fixed_list_order.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v15_RDM-4997_fixed_list_order.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-14060" yWindow="-28340" windowWidth="51200" windowHeight="28340" activeTab="3"/>
+    <workbookView xWindow="-14060" yWindow="-28340" windowWidth="51200" windowHeight="28340" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="579">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1799,15 +1799,6 @@
     <t>GenderField</t>
   </si>
   <si>
-    <t>Class.ClassDetails.ClassLocation.MarritalStatus</t>
-  </si>
-  <si>
-    <t>Class.ClassDetails.ClassLocation.RegionalCentre</t>
-  </si>
-  <si>
-    <t>Class.ClassDetails.ClassLocation.Gender</t>
-  </si>
-  <si>
     <t>School regional centre</t>
   </si>
   <si>
@@ -1866,6 +1857,9 @@
   </si>
   <si>
     <t>classMandatoryForEnum</t>
+  </si>
+  <si>
+    <t>Class.ClassMandatoryFor</t>
   </si>
 </sst>
 </file>
@@ -22475,8 +22469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23729,7 +23723,7 @@
         <v>60</v>
       </c>
       <c r="F38" s="158" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="G38" s="189" t="s">
         <v>547</v>
@@ -24015,16 +24009,16 @@
         <v>435</v>
       </c>
       <c r="D47" s="72" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E47" s="72" t="s">
         <v>62</v>
       </c>
       <c r="F47" s="72" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="G47" s="72" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="H47" s="72"/>
       <c r="I47" s="193"/>
@@ -24179,7 +24173,7 @@
         <v>431</v>
       </c>
       <c r="D52" s="103" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E52" s="104" t="s">
         <v>555</v>
@@ -24188,7 +24182,7 @@
         <v>63</v>
       </c>
       <c r="G52" s="103" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="H52" s="103"/>
       <c r="I52" s="103"/>
@@ -24295,9 +24289,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -24471,7 +24465,7 @@
         <v>454</v>
       </c>
       <c r="F6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -24517,7 +24511,7 @@
         <v>454</v>
       </c>
       <c r="F8" t="s">
-        <v>544</v>
+        <v>578</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -24540,7 +24534,7 @@
         <v>454</v>
       </c>
       <c r="F9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I9">
         <v>3</v>
@@ -24563,7 +24557,7 @@
         <v>454</v>
       </c>
       <c r="F10" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="I10">
         <v>4</v>
@@ -24586,7 +24580,7 @@
         <v>454</v>
       </c>
       <c r="F11" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="I11">
         <v>5</v>
@@ -24609,7 +24603,7 @@
         <v>454</v>
       </c>
       <c r="F12" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="I12">
         <v>6</v>
@@ -24631,14 +24625,14 @@
       <c r="E13" s="84" t="s">
         <v>454</v>
       </c>
-      <c r="F13" t="s">
-        <v>559</v>
+      <c r="F13" s="84" t="s">
+        <v>463</v>
       </c>
       <c r="I13">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J13" s="84" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
@@ -24654,11 +24648,17 @@
       <c r="E14" s="84" t="s">
         <v>454</v>
       </c>
-      <c r="F14" t="s">
-        <v>560</v>
+      <c r="F14" s="84" t="s">
+        <v>465</v>
+      </c>
+      <c r="G14" s="84" t="s">
+        <v>472</v>
+      </c>
+      <c r="H14" s="84" t="s">
+        <v>473</v>
       </c>
       <c r="I14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J14" s="84" t="s">
         <v>439</v>
@@ -24678,13 +24678,13 @@
         <v>454</v>
       </c>
       <c r="F15" s="84" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="I15">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J15" s="84" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
@@ -24701,22 +24701,13 @@
         <v>454</v>
       </c>
       <c r="F16" s="84" t="s">
-        <v>465</v>
-      </c>
-      <c r="G16" s="84" t="s">
-        <v>472</v>
-      </c>
-      <c r="H16" s="84" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="I16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J16" s="84" t="s">
-        <v>439</v>
-      </c>
-      <c r="K16" s="84" t="s">
-        <v>469</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
@@ -24733,13 +24724,16 @@
         <v>454</v>
       </c>
       <c r="F17" s="84" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J17" s="84" t="s">
-        <v>439</v>
+        <v>437</v>
+      </c>
+      <c r="K17" s="84" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
@@ -24756,63 +24750,19 @@
         <v>454</v>
       </c>
       <c r="F18" s="84" t="s">
-        <v>467</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
+        <v>464</v>
       </c>
       <c r="J18" s="84" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A19" s="85">
-        <v>43101</v>
-      </c>
-      <c r="C19" t="s">
-        <v>435</v>
-      </c>
-      <c r="D19" s="84" t="s">
-        <v>452</v>
-      </c>
-      <c r="E19" s="84" t="s">
-        <v>454</v>
-      </c>
-      <c r="F19" s="84" t="s">
-        <v>468</v>
-      </c>
-      <c r="I19">
-        <v>8</v>
-      </c>
-      <c r="J19" s="84" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A20" s="85">
-        <v>43101</v>
-      </c>
-      <c r="C20" t="s">
-        <v>435</v>
-      </c>
-      <c r="D20" s="84" t="s">
-        <v>452</v>
-      </c>
-      <c r="E20" s="84" t="s">
-        <v>454</v>
-      </c>
-      <c r="F20" s="84" t="s">
-        <v>464</v>
-      </c>
-      <c r="J20" s="84" t="s">
-        <v>437</v>
-      </c>
-      <c r="K20" s="84" t="s">
-        <v>470</v>
-      </c>
-    </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="K21" s="84" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="K22" s="84" t="s">
         <v>471</v>
       </c>
     </row>
@@ -25000,13 +24950,13 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="8" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="F8" s="7">
         <v>4</v>
@@ -25022,13 +24972,13 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="8" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -25042,13 +24992,13 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="8" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>562</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>565</v>
       </c>
       <c r="F10" s="7">
         <v>2</v>
@@ -25218,13 +25168,13 @@
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="8" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F19" s="7">
         <v>2</v>
@@ -25236,13 +25186,13 @@
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="8" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F20" s="7">
         <v>4</v>
@@ -25254,13 +25204,13 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="8" t="s">
+        <v>566</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>569</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>572</v>
       </c>
       <c r="F21" s="7">
         <v>5</v>
@@ -25272,13 +25222,13 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="8" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="F22" s="7">
         <v>7</v>
@@ -26846,8 +26796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>